<commit_message>
Adding detailed README and some minor tweaks.
</commit_message>
<xml_diff>
--- a/ddl_tools/test_excel.xlsx
+++ b/ddl_tools/test_excel.xlsx
@@ -1,23 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<s:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <s:workbookPr/>
-  <s:bookViews>
-    <s:workbookView activeTab="0"/>
-  </s:bookViews>
-  <s:sheets>
-    <s:sheet name="Columns" sheetId="1" r:id="rId1"/>
-    <s:sheet name="Tables" sheetId="2" r:id="rId2"/>
-    <s:sheet name="Foreign Keys" sheetId="3" r:id="rId3"/>
-    <s:sheet name="Relationships" sheetId="4" r:id="rId4"/>
-  </s:sheets>
-  <s:definedNames/>
-  <s:calcPr calcId="124519" fullCalcOnLoad="1"/>
-</s:workbook>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bill.back/ThoughtSpot/community-tools/ddl_tools/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="240" yWindow="460" windowWidth="28560" windowHeight="16820" activeTab="1"/>
+  </bookViews>
+  <sheets>
+    <sheet name="Columns" sheetId="1" r:id="rId1"/>
+    <sheet name="Tables" sheetId="2" r:id="rId2"/>
+    <sheet name="Foreign Keys" sheetId="3" r:id="rId3"/>
+    <sheet name="Relationships" sheetId="4" r:id="rId4"/>
+  </sheets>
+  <calcPr calcId="150001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
+</workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="38">
   <si>
     <t>Database</t>
   </si>
@@ -136,14 +149,13 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -165,16 +177,21 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -462,19 +479,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <s:sheetPr>
-    <s:outlinePr summaryBelow="1" summaryRight="1"/>
-  </s:sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -494,7 +506,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -504,7 +516,7 @@
       <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="n">
+      <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
@@ -514,7 +526,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -524,7 +536,7 @@
       <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D3">
         <v>2</v>
       </c>
       <c r="E3" t="s">
@@ -534,7 +546,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -544,7 +556,7 @@
       <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="D4" t="n">
+      <c r="D4">
         <v>3</v>
       </c>
       <c r="E4" t="s">
@@ -554,7 +566,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -564,7 +576,7 @@
       <c r="C5" t="s">
         <v>15</v>
       </c>
-      <c r="D5" t="n">
+      <c r="D5">
         <v>1</v>
       </c>
       <c r="E5" t="s">
@@ -574,7 +586,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -584,7 +596,7 @@
       <c r="C6" t="s">
         <v>15</v>
       </c>
-      <c r="D6" t="n">
+      <c r="D6">
         <v>2</v>
       </c>
       <c r="E6" t="s">
@@ -594,7 +606,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -604,7 +616,7 @@
       <c r="C7" t="s">
         <v>15</v>
       </c>
-      <c r="D7" t="n">
+      <c r="D7">
         <v>3</v>
       </c>
       <c r="E7" t="s">
@@ -614,7 +626,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -624,7 +636,7 @@
       <c r="C8" t="s">
         <v>15</v>
       </c>
-      <c r="D8" t="n">
+      <c r="D8">
         <v>4</v>
       </c>
       <c r="E8" t="s">
@@ -635,24 +647,19 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <s:sheetPr>
-    <s:outlinePr summaryBelow="1" summaryRight="1"/>
-  </s:sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -687,7 +694,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -703,10 +710,9 @@
       <c r="E2" t="s">
         <v>28</v>
       </c>
-      <c r="F2" t="s"/>
       <c r="G2">
         <f>COUNTIFS(Columns!A:A,Tables!A2, Columns!B:B,Tables!B2, Columns!C:C,Tables!C2)</f>
-        <v/>
+        <v>3</v>
       </c>
       <c r="H2" t="s">
         <v>9</v>
@@ -714,12 +720,11 @@
       <c r="I2" t="s">
         <v>9</v>
       </c>
-      <c r="J2" t="n">
+      <c r="J2">
         <v>128</v>
       </c>
-      <c r="K2" t="s"/>
-    </row>
-    <row r="3" spans="1:11">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -735,37 +740,28 @@
       <c r="E3" t="s">
         <v>28</v>
       </c>
-      <c r="F3" t="s"/>
       <c r="G3">
         <f>COUNTIFS(Columns!A:A,Tables!A3, Columns!B:B,Tables!B3, Columns!C:C,Tables!C3)</f>
-        <v/>
+        <v>4</v>
       </c>
       <c r="H3" t="s">
         <v>9</v>
       </c>
-      <c r="I3" t="s"/>
-      <c r="J3" t="s"/>
-      <c r="K3" t="s"/>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <s:sheetPr>
-    <s:outlinePr summaryBelow="1" summaryRight="1"/>
-  </s:sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -788,7 +784,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -812,24 +808,19 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <s:sheetPr>
-    <s:outlinePr summaryBelow="1" summaryRight="1"/>
-  </s:sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -849,7 +840,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -870,6 +861,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added support for enum type conversion.
</commit_message>
<xml_diff>
--- a/ddl_tools/test_excel.xlsx
+++ b/ddl_tools/test_excel.xlsx
@@ -1,36 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bill.back/ThoughtSpot/community-tools/ddl_tools/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="28560" windowHeight="16820" activeTab="1"/>
-  </bookViews>
-  <sheets>
-    <sheet name="Columns" sheetId="1" r:id="rId1"/>
-    <sheet name="Tables" sheetId="2" r:id="rId2"/>
-    <sheet name="Foreign Keys" sheetId="3" r:id="rId3"/>
-    <sheet name="Relationships" sheetId="4" r:id="rId4"/>
-  </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
-</workbook>
+<s:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <s:workbookPr/>
+  <s:bookViews>
+    <s:workbookView activeTab="0"/>
+  </s:bookViews>
+  <s:sheets>
+    <s:sheet name="Columns" sheetId="1" r:id="rId1"/>
+    <s:sheet name="Tables" sheetId="2" r:id="rId2"/>
+    <s:sheet name="Foreign Keys" sheetId="3" r:id="rId3"/>
+    <s:sheet name="Relationships" sheetId="4" r:id="rId4"/>
+  </s:sheets>
+  <s:definedNames/>
+  <s:calcPr calcId="124519" fullCalcOnLoad="1"/>
+</s:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="38">
   <si>
     <t>Database</t>
   </si>
@@ -149,13 +136,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -177,21 +165,16 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -479,14 +462,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <s:sheetPr>
+    <s:outlinePr summaryBelow="1" summaryRight="1"/>
+  </s:sheetPr>
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -506,7 +494,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -516,7 +504,7 @@
       <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="D2">
+      <c r="D2" t="n">
         <v>1</v>
       </c>
       <c r="E2" t="s">
@@ -526,7 +514,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -536,7 +524,7 @@
       <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="D3">
+      <c r="D3" t="n">
         <v>2</v>
       </c>
       <c r="E3" t="s">
@@ -546,7 +534,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -556,7 +544,7 @@
       <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="D4">
+      <c r="D4" t="n">
         <v>3</v>
       </c>
       <c r="E4" t="s">
@@ -566,7 +554,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -576,7 +564,7 @@
       <c r="C5" t="s">
         <v>15</v>
       </c>
-      <c r="D5">
+      <c r="D5" t="n">
         <v>1</v>
       </c>
       <c r="E5" t="s">
@@ -586,7 +574,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -596,7 +584,7 @@
       <c r="C6" t="s">
         <v>15</v>
       </c>
-      <c r="D6">
+      <c r="D6" t="n">
         <v>2</v>
       </c>
       <c r="E6" t="s">
@@ -606,7 +594,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -616,7 +604,7 @@
       <c r="C7" t="s">
         <v>15</v>
       </c>
-      <c r="D7">
+      <c r="D7" t="n">
         <v>3</v>
       </c>
       <c r="E7" t="s">
@@ -626,7 +614,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -636,7 +624,7 @@
       <c r="C8" t="s">
         <v>15</v>
       </c>
-      <c r="D8">
+      <c r="D8" t="n">
         <v>4</v>
       </c>
       <c r="E8" t="s">
@@ -647,19 +635,24 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <s:sheetPr>
+    <s:outlinePr summaryBelow="1" summaryRight="1"/>
+  </s:sheetPr>
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -694,7 +687,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -710,9 +703,10 @@
       <c r="E2" t="s">
         <v>28</v>
       </c>
+      <c r="F2" t="s"/>
       <c r="G2">
         <f>COUNTIFS(Columns!A:A,Tables!A2, Columns!B:B,Tables!B2, Columns!C:C,Tables!C2)</f>
-        <v>3</v>
+        <v/>
       </c>
       <c r="H2" t="s">
         <v>9</v>
@@ -720,11 +714,12 @@
       <c r="I2" t="s">
         <v>9</v>
       </c>
-      <c r="J2">
+      <c r="J2" t="n">
         <v>128</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K2" t="s"/>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -740,28 +735,37 @@
       <c r="E3" t="s">
         <v>28</v>
       </c>
+      <c r="F3" t="s"/>
       <c r="G3">
         <f>COUNTIFS(Columns!A:A,Tables!A3, Columns!B:B,Tables!B3, Columns!C:C,Tables!C3)</f>
-        <v>4</v>
+        <v/>
       </c>
       <c r="H3" t="s">
         <v>9</v>
       </c>
+      <c r="I3" t="s"/>
+      <c r="J3" t="s"/>
+      <c r="K3" t="s"/>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <s:sheetPr>
+    <s:outlinePr summaryBelow="1" summaryRight="1"/>
+  </s:sheetPr>
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -784,7 +788,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -808,19 +812,24 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <s:sheetPr>
+    <s:outlinePr summaryBelow="1" summaryRight="1"/>
+  </s:sheetPr>
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -840,7 +849,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -861,6 +870,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Multiple updates to DDL parser including to support primary, hash, and foreign keys.
</commit_message>
<xml_diff>
--- a/ddl_tools/test_excel.xlsx
+++ b/ddl_tools/test_excel.xlsx
@@ -821,7 +821,7 @@
   <s:sheetPr>
     <s:outlinePr summaryBelow="1" summaryRight="1"/>
   </s:sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -849,23 +849,23 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
         <v>36</v>
       </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
         <v>15</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E3" t="s">
         <v>8</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F3" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updates to convert ddl and adding ddl diff capability.
</commit_message>
<xml_diff>
--- a/ddl_tools/test_excel.xlsx
+++ b/ddl_tools/test_excel.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<s:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <s:workbookPr/>
-  <s:bookViews>
-    <s:workbookView activeTab="0"/>
-  </s:bookViews>
-  <s:sheets>
-    <s:sheet name="Columns" sheetId="1" r:id="rId1"/>
-    <s:sheet name="Tables" sheetId="2" r:id="rId2"/>
-    <s:sheet name="Foreign Keys" sheetId="3" r:id="rId3"/>
-    <s:sheet name="Relationships" sheetId="4" r:id="rId4"/>
-  </s:sheets>
-  <s:definedNames/>
-  <s:calcPr calcId="124519" fullCalcOnLoad="1"/>
-</s:workbook>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
+  <bookViews>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+  </bookViews>
+  <sheets>
+    <sheet name="Columns" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Tables" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Foreign Keys" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Relationships" sheetId="4" state="visible" r:id="rId4"/>
+  </sheets>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+</workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="40">
   <si>
     <t>Database</t>
   </si>
@@ -98,6 +99,12 @@
   </si>
   <si>
     <t>RLS Column</t>
+  </si>
+  <si>
+    <t># FKs From</t>
+  </si>
+  <si>
+    <t># FKs To</t>
   </si>
   <si>
     <t>daily</t>
@@ -149,7 +156,7 @@
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -168,12 +175,11 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
@@ -462,17 +468,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <s:sheetPr>
-    <s:outlinePr summaryBelow="1" summaryRight="1"/>
-  </s:sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
@@ -640,19 +647,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <s:sheetPr>
-    <s:outlinePr summaryBelow="1" summaryRight="1"/>
-  </s:sheetPr>
-  <dimension ref="A1:K3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -686,8 +694,14 @@
       <c r="K1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
+      <c r="L1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -698,10 +712,10 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F2" t="s"/>
       <c r="G2">
@@ -718,8 +732,16 @@
         <v>128</v>
       </c>
       <c r="K2" t="s"/>
-    </row>
-    <row r="3" spans="1:11">
+      <c r="L2">
+        <f>IF(COUNTIF('Foreign Keys'!$D:$D,"="&amp;$C2)&gt;0,COUNTIF('Foreign Keys'!$D:$D,"="&amp;$C2),"")</f>
+        <v/>
+      </c>
+      <c r="M2">
+        <f>IF(COUNTIF('Foreign Keys'!$F:$F,"="&amp;$C2)&gt;0,COUNTIF('Foreign Keys'!$F:$F,"="&amp;$C2),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -730,10 +752,10 @@
         <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F3" t="s"/>
       <c r="G3">
@@ -746,6 +768,14 @@
       <c r="I3" t="s"/>
       <c r="J3" t="s"/>
       <c r="K3" t="s"/>
+      <c r="L3">
+        <f>IF(COUNTIF('Foreign Keys'!$D:$D,"="&amp;$C3)&gt;0,COUNTIF('Foreign Keys'!$D:$D,"="&amp;$C3),"")</f>
+        <v/>
+      </c>
+      <c r="M3">
+        <f>IF(COUNTIF('Foreign Keys'!$F:$F,"="&amp;$C3)&gt;0,COUNTIF('Foreign Keys'!$F:$F,"="&amp;$C3),"")</f>
+        <v/>
+      </c>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
@@ -753,17 +783,18 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <s:sheetPr>
-    <s:outlinePr summaryBelow="1" summaryRight="1"/>
-  </s:sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
@@ -776,21 +807,21 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -805,7 +836,7 @@
         <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G2" t="s">
         <v>9</v>
@@ -817,17 +848,18 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <s:sheetPr>
-    <s:outlinePr summaryBelow="1" summaryRight="1"/>
-  </s:sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
@@ -840,18 +872,18 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -866,7 +898,7 @@
         <v>8</v>
       </c>
       <c r="F3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>